<commit_message>
memory demand analysis data collected
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_Action.xlsx
+++ b/projects/test_building/input/ID_Action.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FE0067-9259-D84E-A329-F07E05FD2E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92824273-8E67-8D4C-8375-C3DB697A4ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5640" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -28,9 +28,6 @@
     <t>building - new construction</t>
   </si>
   <si>
-    <t>building - refurbishment</t>
-  </si>
-  <si>
     <t>technology - new installation</t>
   </si>
   <si>
@@ -41,6 +38,12 @@
   </si>
   <si>
     <t>id_action</t>
+  </si>
+  <si>
+    <t>building - conventional renovation</t>
+  </si>
+  <si>
+    <t>building - serial renovation</t>
   </si>
 </sst>
 </file>
@@ -96,8 +99,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_action"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
@@ -369,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="188" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -383,7 +386,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -402,7 +405,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -410,7 +413,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -418,7 +421,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -426,7 +429,15 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>